<commit_message>
curves: some first part of the user pipeline
</commit_message>
<xml_diff>
--- a/input/curves/dsc.1/data.xlsx
+++ b/input/curves/dsc.1/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\curves\dsc.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E88F0-038D-495F-857D-A6D750B02F36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36C57AB-E980-42A3-97F6-C075696208F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>median</t>
-  </si>
-  <si>
     <t>hwhm</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>gaussian</t>
+  </si>
+  <si>
+    <t>expvalue</t>
   </si>
 </sst>
 </file>
@@ -405,10 +405,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4590,7 +4590,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4606,21 +4606,21 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4628,15 +4628,15 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>350</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4644,13 +4644,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4658,10 +4658,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
       </c>
       <c r="D6">
         <v>230</v>
@@ -4672,13 +4672,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,13 +4686,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4700,10 +4700,10 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
       </c>
       <c r="D9">
         <v>300</v>
@@ -4714,13 +4714,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
curves : sanitze parameters input
</commit_message>
<xml_diff>
--- a/input/curves/dsc.1/data.xlsx
+++ b/input/curves/dsc.1/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\curves\dsc.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36C57AB-E980-42A3-97F6-C075696208F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE02CF60-E486-4040-BA9B-3DFB72AF3FE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4590,7 +4590,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
curves : another synchronization issue (updating formula inputs w/o rewriting dt.par with older values)
</commit_message>
<xml_diff>
--- a/input/curves/dsc.1/data.xlsx
+++ b/input/curves/dsc.1/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\data science\chemistry\kev\input\curves\dsc.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE02CF60-E486-4040-BA9B-3DFB72AF3FE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340B9A8-0217-44CC-A2A9-E6C23D886E43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4590,7 +4590,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>

</xml_diff>